<commit_message>
Added after the seminar
</commit_message>
<xml_diff>
--- a/Resource/data.xlsx
+++ b/Resource/data.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/s_raina_dxc_com/Documents/Desktop/FilloPractice/Resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{D56DB78C-E5BA-45A0-B38F-8CEEDDFB65E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA69CF87-84E5-409E-80DD-2F92147E64D1}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{D56DB78C-E5BA-45A0-B38F-8CEEDDFB65E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3A11DAE-37ED-432B-8C00-3B7EA94958E9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD285DBD-5499-471D-BF84-186954332DA0}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>TC</t>
   </si>
@@ -53,12 +53,28 @@
   </si>
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>US</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,46 +432,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.453125" customWidth="1"/>
-    <col min="2" max="2" width="16.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="11.453125"/>
+    <col min="2" max="2" customWidth="true" width="16.08984375"/>
+    <col min="3" max="3" customWidth="true" width="15.26953125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>4</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>6</v>
       </c>
+      <c r="D3" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -464,23 +484,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6275FE2-32C2-47AE-9FB3-D1715B50713D}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>